<commit_message>
change in spreadsheet and README files
</commit_message>
<xml_diff>
--- a/spreadsheet_template.xlsx
+++ b/spreadsheet_template.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="project" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="sample" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="experiment" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="run" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="project" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="sample" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="experiment" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="run" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <t xml:space="preserve">alias</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">sample_description</t>
   </si>
   <si>
+    <t xml:space="preserve">collection date</t>
+  </si>
+  <si>
     <t xml:space="preserve">collected_by</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Natural diploid yeast isolated from Lunar soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-01-23</t>
   </si>
   <si>
     <t xml:space="preserve">Lunar Rover 1</t>
@@ -209,15 +215,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-40C];[RED]\-#,##0.00\ [$€-40C]"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -239,14 +247,21 @@
       <sz val="10"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF6D"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -282,10 +297,24 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,11 +328,177 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Résultat2" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF6D"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -315,30 +510,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="74.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -354,128 +549,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="34.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>4932</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>4932</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>4932</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -490,154 +694,154 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="35.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="35.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="H3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="L2" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -652,7 +856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -664,61 +868,61 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="23.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="23.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>59</v>
+      <c r="D3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
take care of optional columns in the spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet_template.xlsx
+++ b/spreadsheet_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,8 +22,116 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Frédéric BIGEY</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">free text</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">free text</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Frédéric BIGEY</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NCBI taxid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">YYYY-MM-DD
+not applicable
+not collected
+not provided</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Country
+not applicable
+not collected
+not provided</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Frédéric BIGEY</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">yes|no</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t xml:space="preserve">alias</t>
   </si>
@@ -82,6 +190,9 @@
     <t xml:space="preserve">Saccharomyces cerevisiae</t>
   </si>
   <si>
+    <t xml:space="preserve">Baker’s yeast</t>
+  </si>
+  <si>
     <t xml:space="preserve">MTF0000</t>
   </si>
   <si>
@@ -94,10 +205,10 @@
     <t xml:space="preserve">Lunar Rover 1</t>
   </si>
   <si>
-    <t xml:space="preserve">not provided</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil</t>
+    <t xml:space="preserve">Moon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free text</t>
   </si>
   <si>
     <t xml:space="preserve">sam_0001</t>
@@ -220,7 +331,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-40C];[RED]\-#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -249,13 +360,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -301,7 +423,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,8 +436,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -504,25 +638,25 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="74.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="78.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -545,6 +679,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -555,36 +690,37 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -596,13 +732,13 @@
       <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -625,34 +761,37 @@
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>4932</v>
@@ -660,26 +799,29 @@
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -690,6 +832,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -701,7 +844,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,10 +857,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="35.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="37.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.62"/>
   </cols>
   <sheetData>
@@ -729,45 +872,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -776,72 +919,72 @@
         <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="I2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="5" t="n">
         <v>300</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="5" t="n">
         <v>30</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="I3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="5" t="n">
         <v>300</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="5" t="n">
         <v>30</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -852,6 +995,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -863,66 +1007,66 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="23.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
possibility to leave some sheet blank if already declared
</commit_message>
<xml_diff>
--- a/spreadsheet_template.xlsx
+++ b/spreadsheet_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" state="visible" r:id="rId3"/>
@@ -62,6 +62,30 @@
     <author>Frédéric BIGEY</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">give an unique id for each samples</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">free text</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C1" authorId="0">
       <text>
         <r>
@@ -114,6 +138,104 @@
     <author>Frédéric BIGEY</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">give an unique id for each experiements (library construction)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">free text</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Internal project ID or BioProject accession number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">internal (declared in sample sheet) or accession (already declared at EBI)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Internal sample ID or BioSample accession number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">internal or accession</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Internal library name
+Must be unique</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">WGS
+RNA-Seq</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I1" authorId="0">
       <text>
         <r>
@@ -122,7 +244,110 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">GENOMIC
+TRANSCRIPTOMIC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">size fractionation
+cDNA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">yes|no</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">free text</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ILLUMINA
+BGISEQ
+OXFORD_NANOPORE
+PACBIO_SMRT
+ION_TORRENT
+CAPILLARY</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Illumina HiSeq 2000
+GridION
+unspecified</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Frédéric BIGEY</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">give an internal unique ID for each runs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Internal experiement ID </t>
         </r>
       </text>
     </comment>
@@ -131,9 +356,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
-  <si>
-    <t xml:space="preserve">alias</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
+  <si>
+    <t xml:space="preserve">Project ID</t>
   </si>
   <si>
     <t xml:space="preserve">TITLE</t>
@@ -151,34 +376,40 @@
     <t xml:space="preserve">This study aimed to characterise the microbial diversity of yeasts isolated from Lunar soils</t>
   </si>
   <si>
-    <t xml:space="preserve">TAXON_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCIENTIFIC_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMMON_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collection date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collected_by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geographic location (country and/or sea)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geographic location (region and locality)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isolation_source</t>
+    <t xml:space="preserve">Sample ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxon ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scientific name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collection date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collected by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geographic location (country and/or sea)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geographic location (region and locality)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isolation source</t>
   </si>
   <si>
     <t xml:space="preserve">sam_0000</t>
@@ -223,37 +454,49 @@
     <t xml:space="preserve">Lunar Rover 2</t>
   </si>
   <si>
-    <t xml:space="preserve">STUDY_REF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMPLE_DESCRIPTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIBRARY_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIBRARY_STRATEGY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIBRARY_SOURCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIBRARY_SELECTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAIRED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOMINAL_LENGTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOMINAL_SDEV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIBRARY_CONSTRUCTION_PROTOCOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSTRUMENT_MODEL</t>
+    <t xml:space="preserve">Experiment ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert size SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library construction protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instrument model</t>
   </si>
   <si>
     <t xml:space="preserve">exp_0000</t>
@@ -262,6 +505,9 @@
     <t xml:space="preserve">Lunar yeast sequencing project</t>
   </si>
   <si>
+    <t xml:space="preserve">internal</t>
+  </si>
+  <si>
     <t xml:space="preserve">lib_0000</t>
   </si>
   <si>
@@ -280,6 +526,9 @@
     <t xml:space="preserve">Library construction protocol here</t>
   </si>
   <si>
+    <t xml:space="preserve">Illumina</t>
+  </si>
+  <si>
     <t xml:space="preserve">Illumina HiSeq 2000</t>
   </si>
   <si>
@@ -289,7 +538,10 @@
     <t xml:space="preserve">lib_0001</t>
   </si>
   <si>
-    <t xml:space="preserve">EXPERIMENT_REF</t>
+    <t xml:space="preserve">Run ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment reference</t>
   </si>
   <si>
     <t xml:space="preserve">filetype</t>
@@ -638,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -690,8 +942,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,7 +955,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.33"/>
@@ -712,116 +964,116 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>4932</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>4932</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -841,150 +1093,179 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="37.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="37.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="20.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="5" t="n">
         <v>300</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="M2" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>49</v>
+      <c r="N2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="5" t="n">
+      <c r="I3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="5" t="n">
         <v>300</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="M3" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>49</v>
+      <c r="N3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1020,53 +1301,53 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1077,5 +1358,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in README, spreadsheet and python script
</commit_message>
<xml_diff>
--- a/spreadsheet_template.xlsx
+++ b/spreadsheet_template.xlsx
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -356,32 +356,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="100">
   <si>
     <t xml:space="preserve">Project ID</t>
   </si>
   <si>
-    <t xml:space="preserve">TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proj_0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity of yeast isolated from Lunar soils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This study aimed to characterise the microbial diversity of yeasts isolated from Lunar soils</t>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
   </si>
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
     <t xml:space="preserve">Taxon ID</t>
   </si>
   <si>
@@ -394,6 +382,9 @@
     <t xml:space="preserve">Strain</t>
   </si>
   <si>
+    <t xml:space="preserve">Culture collection</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample description</t>
   </si>
   <si>
@@ -415,43 +406,34 @@
     <t xml:space="preserve">sam_0000</t>
   </si>
   <si>
-    <t xml:space="preserve">Saccharomyces cerevisiae strain MTF0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saccharomyces cerevisiae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baker’s yeast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTF0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural diploid yeast isolated from Lunar soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-01-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lunar Rover 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">free text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sam_0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saccharomyces cerevisiae strain MTF0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTF0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lunar Rover 2</t>
+    <t xml:space="preserve">Trichomonascus vanleenenianus  strain CLIB 3782 (synonym L1-24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trichomonascus vanleenenianus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIB 3782</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIB:3782</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural haploid yeast isolated from the gut of insect larvae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anita Boisramé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Essarts-le-roi (F-78690)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gut of insect larvae</t>
   </si>
   <si>
     <t xml:space="preserve">Experiment ID</t>
@@ -502,15 +484,36 @@
     <t xml:space="preserve">exp_0000</t>
   </si>
   <si>
-    <t xml:space="preserve">Lunar yeast sequencing project</t>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trichomonascus vanleenenianus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> CLIB 3782 sequencing project</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJEB90485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accession</t>
   </si>
   <si>
     <t xml:space="preserve">internal</t>
   </si>
   <si>
-    <t xml:space="preserve">lib_0000</t>
-  </si>
-  <si>
     <t xml:space="preserve">WGS</t>
   </si>
   <si>
@@ -526,16 +529,106 @@
     <t xml:space="preserve">Library construction protocol here</t>
   </si>
   <si>
-    <t xml:space="preserve">Illumina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Illumina HiSeq 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exp_0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lib_0001</t>
+    <t xml:space="preserve">DNBSEQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unspecified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_G24_1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trichomonascus vanleenenianus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CLIB 3782 mRNA sequencing after 24 hours of growth on YNB glucose</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">G24_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA-seq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSCRIPTOMIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oligo-dT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strand-specific cDNA library construction: mRNA fragmentation, Random primed cDNA synthesis, Adapter ligation and adapter specific PCR amplification. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILLUMINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina NovaSeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_G24_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G24_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_G24_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G24_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_X24_1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trichomonascus vanleenenianus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CLIB 3782 mRNA sequencing after 24 hours of growth on YNB xylan</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">X24_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_X24_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X24_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_X24_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X24_3</t>
   </si>
   <si>
     <t xml:space="preserve">Run ID</t>
@@ -559,19 +652,64 @@
     <t xml:space="preserve">fastq</t>
   </si>
   <si>
-    <t xml:space="preserve">read_0000_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read_0000_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read_0001_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read_0001_R2.fastq.gz</t>
+    <t xml:space="preserve">L1-24_1.fq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1-24_2.fq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_G24_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_G24_1_libLAI6747_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_G24_1_libLAI6747_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_G24_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_G24_2_libLAI6746_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_G24_2_libLAI6746_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_G24_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_G24_3_libLAI6748_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_G24_3_libLAI6748_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_X24_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_X24_1_libLAI6749_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_X24_1_libLAI6749_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_X24_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_X24_2_libLAI6750_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_X24_2_libLAI6750_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_X24_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_X24_3_libLAI6751_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG-A2732_X24_3_libLAI6751_2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -583,7 +721,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-40C];[RED]\-#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -616,6 +754,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -675,7 +820,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -692,16 +837,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -888,10 +1041,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,17 +1063,6 @@
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -940,141 +1082,110 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="51.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="35.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="34.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2268995</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>4932</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>4932</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="I3" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1093,24 +1204,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.28"/>
@@ -1120,152 +1231,378 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="K2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="N2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="K3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="L3" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="L4" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="O4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>57</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1285,10 +1622,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1296,58 +1633,143 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="23.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="35.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="C7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comments in spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet_template.xlsx
+++ b/spreadsheet_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,6 +28,18 @@
     <author>Frédéric BIGEY</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">internal ID of the project</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -70,7 +82,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">give an unique id for each samples</t>
+          <t xml:space="preserve">internal ID for the sample</t>
         </r>
       </text>
     </comment>
@@ -98,6 +110,67 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">registered scientific name of the organism</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">free text</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">strain name/id</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Institution code and culture ID are separated by a colon
+eg: CBS:123</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">free text</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I1" authorId="0">
       <text>
         <r>
@@ -107,12 +180,26 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">YYYY-MM-DD
+YYYY-MM
+YYYY
 not applicable
 not collected
 not provided</t>
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">name of the person who isolated/collected the sample</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K1" authorId="0">
       <text>
         <r>
@@ -121,10 +208,35 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Country
+          <t xml:space="preserve">geographical origin of the sample as defined by the country
+Country
 not applicable
 not collected
 not provided</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">geographic origin of the sample as defined by the specific region name followed by the locality name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">physical, environmental and/or local geographical source of the biological sample from which the sample was derived</t>
         </r>
       </text>
     </comment>
@@ -146,7 +258,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">give an unique id for each experiements (library construction)</t>
+          <t xml:space="preserve">internal ID for the experiement</t>
         </r>
       </text>
     </comment>
@@ -182,31 +294,31 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">internal (declared in project sheet) or accession (project already declared at EBI)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Internal sample ID or BioSample accession number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">internal (declared in sample sheet) or accession (already declared at EBI)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Internal sample ID or BioSample accession number</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">internal or accession</t>
         </r>
       </text>
     </comment>
@@ -231,8 +343,8 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">WGS
-RNA-Seq</t>
+          <t xml:space="preserve">Permitted values (see documentations)
+eg: WGS,RNA-Seq</t>
         </r>
       </text>
     </comment>
@@ -244,7 +356,8 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">GENOMIC
+          <t xml:space="preserve">Permitted values (see documentation)
+eg: GENOMIC,
 TRANSCRIPTOMIC</t>
         </r>
       </text>
@@ -257,8 +370,8 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">size fractionation
-cDNA</t>
+          <t xml:space="preserve">Permitted values (see documentation)
+eg: size fractionation, cDNA</t>
         </r>
       </text>
     </comment>
@@ -270,7 +383,32 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">yes|no</t>
+          <t xml:space="preserve">is sequencing paired?
+yes or no</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">insert size (bp)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">insert size standard deviation</t>
         </r>
       </text>
     </comment>
@@ -294,7 +432,9 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">ILLUMINA
+          <t xml:space="preserve">Sequencing platform. Permitted values (see documentation)
+eg:
+ILLUMINA
 BGISEQ
 OXFORD_NANOPORE
 PACBIO_SMRT
@@ -311,7 +451,9 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Illumina HiSeq 2000
+          <t xml:space="preserve">Instrument model. Permitted values (see documentation)
+eg:
+Illumina HiSeq 2000
 GridION
 unspecified</t>
         </r>
@@ -335,7 +477,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">give an internal unique ID for each runs</t>
+          <t xml:space="preserve">internal ID for the run</t>
         </r>
       </text>
     </comment>
@@ -347,7 +489,46 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Internal experiement ID </t>
+          <t xml:space="preserve">internal experiement ID (see experiment sheet)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">file format
+BAM
+CRAM
+FASTQ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">read name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">read name</t>
         </r>
       </text>
     </comment>
@@ -706,7 +887,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -952,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -962,7 +1143,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="51.61"/>
@@ -1030,7 +1211,6 @@
       <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="0"/>
       <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1060,7 +1240,6 @@
       <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="0"/>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1099,7 +1278,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.9"/>
@@ -1183,10 +1362,10 @@
       <c r="E2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1233,10 +1412,10 @@
       <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1313,7 +1492,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>